<commit_message>
Data cleaning & preparation et commentaires ajoutés
</commit_message>
<xml_diff>
--- a/DATA/FINAL_DATASET.xlsx
+++ b/DATA/FINAL_DATASET.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CADENET Margaux\FINAL_PROJECT_Advanced Statistics for Data Science_\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CADENET Margaux\FINAL_PYTHON_PROJECT\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E381CBEF-B47E-4ACF-9200-6670565A7692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55F1B37-FFED-4B1B-9334-F7F53299DA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{F7009158-E7E3-41D8-A23E-8969245B27D9}"/>
   </bookViews>
@@ -2747,13 +2747,13 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2859,11 +2859,11 @@
     <tableColumn id="5" xr3:uid="{D3708CEE-B3D3-4F8A-9B20-9AC2501B3C1C}" uniqueName="5" name="FONCTION" queryTableFieldId="5" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{F3E88C87-70DC-45E5-9C47-9E3EEBC650D5}" uniqueName="6" name="ANCIENNETE" queryTableFieldId="6"/>
     <tableColumn id="7" xr3:uid="{2E1CF7C4-4C60-4DE3-8DA7-09EA35A40134}" uniqueName="7" name="AGE" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{2193CEAF-477E-41AA-A5A6-5C613015AAB4}" uniqueName="8" name="SEX" queryTableFieldId="8" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{2193CEAF-477E-41AA-A5A6-5C613015AAB4}" uniqueName="8" name="SEX" queryTableFieldId="8" dataDxfId="2"/>
     <tableColumn id="9" xr3:uid="{3262A321-8DA2-466B-B89A-14F2879E511F}" uniqueName="9" name="SITUFAM" queryTableFieldId="9"/>
-    <tableColumn id="10" xr3:uid="{CEF6197D-BE5A-44E9-8181-2D711B4EDCE1}" uniqueName="10" name="NBENFANT" queryTableFieldId="10" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{CEF6197D-BE5A-44E9-8181-2D711B4EDCE1}" uniqueName="10" name="NBENFANT" queryTableFieldId="10" dataDxfId="1"/>
     <tableColumn id="11" xr3:uid="{AAD7DCBE-665F-4D24-91DE-91FACD3AC1C3}" uniqueName="11" name="NIVEAUETUDE" queryTableFieldId="11"/>
-    <tableColumn id="12" xr3:uid="{4CCBDB8F-22CB-4071-95EE-5010DA9EE0A9}" uniqueName="12" name="FORMATION" queryTableFieldId="12" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{4CCBDB8F-22CB-4071-95EE-5010DA9EE0A9}" uniqueName="12" name="FORMATION" queryTableFieldId="12" dataDxfId="0"/>
     <tableColumn id="13" xr3:uid="{7CEE93B9-E61F-444A-8078-B926DAC3979F}" uniqueName="13" name="MHCB1" queryTableFieldId="13"/>
     <tableColumn id="14" xr3:uid="{CACC3707-7D25-42C9-8AEE-56B38BFD54B8}" uniqueName="14" name="MHCC1" queryTableFieldId="14"/>
     <tableColumn id="15" xr3:uid="{CB3F2C3E-D73F-45F3-9960-FAD6D86DB439}" uniqueName="15" name="MHCB2" queryTableFieldId="15"/>
@@ -3218,8 +3218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BCBBB36-9A01-43DB-9C96-F9EAA779BDAE}">
   <dimension ref="A1:BK318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AL1" sqref="AL1:AL1048576"/>
+    <sheetView tabSelected="1" topLeftCell="N91" workbookViewId="0">
+      <selection activeCell="U110" sqref="U110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>